<commit_message>
updating country status in excel file
</commit_message>
<xml_diff>
--- a/resources/tests_urls_tips_final.xlsx
+++ b/resources/tests_urls_tips_final.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="508">
   <si>
     <t>country</t>
   </si>
@@ -1551,9 +1551,6 @@
     <t>twitter information</t>
   </si>
   <si>
-    <t>to be implemented</t>
-  </si>
-  <si>
     <t>not yet implemented</t>
   </si>
   <si>
@@ -1563,13 +1560,22 @@
     <t>stauts_with_automatization</t>
   </si>
   <si>
-    <t>We're fixing errors in python</t>
-  </si>
-  <si>
     <t>We need to review the new link</t>
   </si>
   <si>
     <t>withuot info, We need to check with new links</t>
+  </si>
+  <si>
+    <t>https://www.nicd.ac.za/diseases-a-z-index/covid-19/surveillance-reports/national-covid-19-daily-report/</t>
+  </si>
+  <si>
+    <t>automated, but need some checks</t>
+  </si>
+  <si>
+    <t>automated Selenium but need some checks</t>
+  </si>
+  <si>
+    <t>not yet implemented, needs an additional step</t>
   </si>
 </sst>
 </file>
@@ -1858,7 +1864,7 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -2146,10 +2152,10 @@
   <dimension ref="A1:L182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2164,6 +2170,7 @@
     <col min="9" max="9" width="61.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="61.5703125" style="2" customWidth="1"/>
     <col min="11" max="11" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2201,7 +2208,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="41" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2258,7 +2265,7 @@
         <v>470</v>
       </c>
       <c r="L3" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2277,8 +2284,8 @@
       <c r="H4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
-        <v>503</v>
+      <c r="L4" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2297,8 +2304,8 @@
       <c r="H5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L5" t="s">
-        <v>503</v>
+      <c r="L5" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2381,7 +2388,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="7"/>
       <c r="L8" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2403,7 +2410,7 @@
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
-      <c r="L9" t="s">
+      <c r="L9" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2428,7 +2435,7 @@
       </c>
       <c r="K10" s="7"/>
       <c r="L10" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2449,7 +2456,7 @@
       </c>
       <c r="K11" s="7"/>
       <c r="L11" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2473,7 +2480,7 @@
       </c>
       <c r="K12" s="7"/>
       <c r="L12" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2494,7 +2501,7 @@
         <v>389</v>
       </c>
       <c r="L13" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2514,7 +2521,7 @@
         <v>390</v>
       </c>
       <c r="L14" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2542,7 +2549,7 @@
         <v>391</v>
       </c>
       <c r="L15" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2565,7 +2572,7 @@
         <v>392</v>
       </c>
       <c r="L16" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2606,7 +2613,7 @@
       <c r="H18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2630,7 +2637,7 @@
       <c r="H19" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2674,7 +2681,7 @@
         <v>393</v>
       </c>
       <c r="L21" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2694,7 +2701,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="7"/>
-      <c r="L22" t="s">
+      <c r="L22" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2714,8 +2721,8 @@
       <c r="H23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L23" t="s">
-        <v>503</v>
+      <c r="L23" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2735,7 +2742,7 @@
       <c r="H24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2755,8 +2762,8 @@
         <v>17</v>
       </c>
       <c r="K25" s="7"/>
-      <c r="L25" t="s">
-        <v>496</v>
+      <c r="L25" s="10" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -2776,7 +2783,7 @@
         <v>255</v>
       </c>
       <c r="I26"/>
-      <c r="L26" t="s">
+      <c r="L26" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2796,7 +2803,7 @@
       <c r="H27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2816,7 +2823,7 @@
       <c r="H28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2835,7 +2842,7 @@
       </c>
       <c r="H29" s="4"/>
       <c r="L29" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2854,7 +2861,7 @@
       <c r="H30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2875,7 +2882,7 @@
         <v>17</v>
       </c>
       <c r="K31" s="7"/>
-      <c r="L31" t="s">
+      <c r="L31" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2895,8 +2902,8 @@
       <c r="H32" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L32" t="s">
-        <v>503</v>
+      <c r="L32" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2915,7 +2922,7 @@
       <c r="H33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L33" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2935,7 +2942,7 @@
       <c r="H34" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2963,7 +2970,7 @@
         <v>60556</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" t="s">
+      <c r="L35" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -2988,7 +2995,7 @@
       </c>
       <c r="K36" s="7"/>
       <c r="L36" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -3007,7 +3014,7 @@
       <c r="H37" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3052,7 +3059,7 @@
       <c r="H39" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L39" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3076,7 +3083,7 @@
         <v>394</v>
       </c>
       <c r="K40" s="8"/>
-      <c r="L40" t="s">
+      <c r="L40" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3103,7 +3110,7 @@
         <v>395</v>
       </c>
       <c r="L41" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -3127,7 +3134,7 @@
         <v>81</v>
       </c>
       <c r="L42" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -3147,7 +3154,7 @@
         <v>85</v>
       </c>
       <c r="K43" s="7"/>
-      <c r="L43" t="s">
+      <c r="L43" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3167,7 +3174,7 @@
       <c r="H44" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L44" t="s">
+      <c r="L44" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3194,7 +3201,7 @@
         <v>397</v>
       </c>
       <c r="L45" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -3213,7 +3220,7 @@
       <c r="H46" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L46" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3273,7 +3280,7 @@
         <v>429</v>
       </c>
       <c r="I49"/>
-      <c r="L49" t="s">
+      <c r="L49" s="41" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3293,7 +3300,7 @@
       <c r="H50" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L50" t="s">
+      <c r="L50" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3316,7 +3323,7 @@
       <c r="K51" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L51" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3342,7 +3349,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="2"/>
       <c r="K52"/>
-      <c r="L52" t="s">
+      <c r="L52" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3362,7 +3369,7 @@
       <c r="H53" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L53" t="s">
+      <c r="L53" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3386,7 +3393,7 @@
         <v>14</v>
       </c>
       <c r="I54" s="36"/>
-      <c r="L54" t="s">
+      <c r="L54" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3406,8 +3413,8 @@
       <c r="H55" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L55" t="s">
-        <v>503</v>
+      <c r="L55" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3426,7 +3433,7 @@
       <c r="H56" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L56" t="s">
+      <c r="L56" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3447,7 +3454,7 @@
       <c r="H57" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L57" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3468,7 +3475,7 @@
         <v>398</v>
       </c>
       <c r="L58" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3494,7 +3501,7 @@
         <v>406</v>
       </c>
       <c r="I59" s="30"/>
-      <c r="L59" t="s">
+      <c r="L59" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3516,7 +3523,7 @@
         <v>121</v>
       </c>
       <c r="K60" s="7"/>
-      <c r="L60" t="s">
+      <c r="L60" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3536,7 +3543,7 @@
       </c>
       <c r="K61" s="7"/>
       <c r="L61" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -3555,7 +3562,7 @@
       <c r="H62" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L62" t="s">
+      <c r="L62" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3574,7 +3581,7 @@
       </c>
       <c r="H63" s="4"/>
       <c r="L63" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -3614,7 +3621,7 @@
       <c r="H65" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L65" t="s">
+      <c r="L65" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3656,7 +3663,7 @@
       <c r="H67" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="L67" t="s">
+      <c r="L67" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3696,7 +3703,7 @@
       <c r="K69" t="s">
         <v>402</v>
       </c>
-      <c r="L69" t="s">
+      <c r="L69" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3716,8 +3723,8 @@
       <c r="H70" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L70" t="s">
-        <v>503</v>
+      <c r="L70" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -3736,7 +3743,7 @@
       <c r="H71" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L71" t="s">
+      <c r="L71" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3773,7 +3780,7 @@
       </c>
       <c r="H73" s="4"/>
       <c r="L73" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -3817,7 +3824,7 @@
         <v>121</v>
       </c>
       <c r="K75" s="7"/>
-      <c r="L75" t="s">
+      <c r="L75" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3839,7 +3846,7 @@
       <c r="K76" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="L76" t="s">
+      <c r="L76" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3866,7 +3873,7 @@
       <c r="H77" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L77" t="s">
+      <c r="L77" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3888,7 +3895,7 @@
         <v>129</v>
       </c>
       <c r="K78" s="7"/>
-      <c r="L78" t="s">
+      <c r="L78" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3910,7 +3917,7 @@
         <v>403</v>
       </c>
       <c r="L79" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -3931,7 +3938,7 @@
         <v>404</v>
       </c>
       <c r="L80" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -3952,7 +3959,7 @@
         <v>17</v>
       </c>
       <c r="K81" s="7"/>
-      <c r="L81" t="s">
+      <c r="L81" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3998,7 +4005,7 @@
       </c>
       <c r="K83" s="7"/>
       <c r="L83" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -4026,7 +4033,7 @@
       <c r="K84" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="L84" t="s">
+      <c r="L84" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4047,7 +4054,7 @@
       <c r="K85" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="L85" t="s">
+      <c r="L85" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4070,7 +4077,7 @@
       </c>
       <c r="K86" s="7"/>
       <c r="L86" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -4090,7 +4097,7 @@
         <v>408</v>
       </c>
       <c r="L87" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -4109,7 +4116,7 @@
       <c r="H88" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L88" t="s">
+      <c r="L88" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4152,7 +4159,7 @@
       <c r="I90"/>
       <c r="K90" s="7"/>
       <c r="L90" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -4174,7 +4181,7 @@
       <c r="I91"/>
       <c r="K91" s="7"/>
       <c r="L91" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -4195,7 +4202,7 @@
         <v>121</v>
       </c>
       <c r="K92" s="7"/>
-      <c r="L92" t="s">
+      <c r="L92" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4222,7 +4229,7 @@
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
       <c r="L93" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -4241,8 +4248,8 @@
       <c r="H94" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L94" t="s">
-        <v>503</v>
+      <c r="L94" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -4261,7 +4268,7 @@
       <c r="H95" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L95" t="s">
+      <c r="L95" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4281,7 +4288,7 @@
       <c r="H96" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L96" t="s">
+      <c r="L96" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4303,7 +4310,7 @@
       </c>
       <c r="I97" s="36"/>
       <c r="K97" s="8"/>
-      <c r="L97" t="s">
+      <c r="L97" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4328,7 +4335,7 @@
         <v>410</v>
       </c>
       <c r="L98" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="99" spans="1:12">
@@ -4347,8 +4354,8 @@
       <c r="H99" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L99" t="s">
-        <v>503</v>
+      <c r="L99" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -4363,7 +4370,7 @@
       </c>
       <c r="H100" s="4"/>
       <c r="L100" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -4382,7 +4389,7 @@
       <c r="H101" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L101" t="s">
+      <c r="L101" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4404,7 +4411,7 @@
         <v>444</v>
       </c>
       <c r="L102" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -4423,7 +4430,7 @@
       <c r="H103" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L103" t="s">
+      <c r="L103" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4447,7 +4454,7 @@
         <v>411</v>
       </c>
       <c r="L104" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="105" spans="1:12">
@@ -4466,7 +4473,7 @@
       <c r="H105" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L105" t="s">
+      <c r="L105" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4486,8 +4493,8 @@
       <c r="H106" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L106" t="s">
-        <v>503</v>
+      <c r="L106" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="107" spans="1:12">
@@ -4509,7 +4516,7 @@
         <v>412</v>
       </c>
       <c r="L107" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
     </row>
     <row r="108" spans="1:12">
@@ -4530,7 +4537,7 @@
       <c r="I108"/>
       <c r="K108" s="8"/>
       <c r="L108" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -4551,7 +4558,7 @@
       <c r="I109"/>
       <c r="K109" s="7"/>
       <c r="L109" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -4570,8 +4577,8 @@
       <c r="H110" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L110" t="s">
-        <v>503</v>
+      <c r="L110" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -4590,8 +4597,8 @@
       <c r="H111" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L111" t="s">
-        <v>503</v>
+      <c r="L111" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="112" spans="1:12">
@@ -4611,7 +4618,7 @@
         <v>413</v>
       </c>
       <c r="L112" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="113" spans="1:12">
@@ -4630,8 +4637,8 @@
       <c r="H113" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L113" t="s">
-        <v>503</v>
+      <c r="L113" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="114" spans="1:12">
@@ -4652,8 +4659,8 @@
       </c>
       <c r="I114" s="5"/>
       <c r="J114" s="6"/>
-      <c r="L114" t="s">
-        <v>496</v>
+      <c r="L114" s="10" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="115" spans="1:12">
@@ -4676,7 +4683,7 @@
         <v>414</v>
       </c>
       <c r="L115" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -4698,7 +4705,7 @@
         <v>256</v>
       </c>
       <c r="L116" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -4719,7 +4726,7 @@
         <v>17</v>
       </c>
       <c r="K117" s="7"/>
-      <c r="L117" t="s">
+      <c r="L117" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4739,7 +4746,7 @@
       <c r="H118" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L118" t="s">
+      <c r="L118" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4759,7 +4766,7 @@
       <c r="H119" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L119" t="s">
+      <c r="L119" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4781,7 +4788,7 @@
         <v>121</v>
       </c>
       <c r="I120" s="36"/>
-      <c r="L120" t="s">
+      <c r="L120" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4803,7 +4810,7 @@
       <c r="H121" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L121" t="s">
+      <c r="L121" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4824,7 +4831,7 @@
         <v>17</v>
       </c>
       <c r="K122" s="7"/>
-      <c r="L122" t="s">
+      <c r="L122" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4864,8 +4871,8 @@
         <v>17</v>
       </c>
       <c r="I124" s="36"/>
-      <c r="L124" t="s">
-        <v>496</v>
+      <c r="L124" s="10" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="125" spans="1:12">
@@ -4908,7 +4915,7 @@
       <c r="I126" s="36"/>
       <c r="K126" s="7"/>
       <c r="L126" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="127" spans="1:12">
@@ -4926,7 +4933,7 @@
       </c>
       <c r="K127" s="7"/>
       <c r="L127" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -4954,7 +4961,7 @@
       </c>
       <c r="I128" s="4"/>
       <c r="L128" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -4973,7 +4980,7 @@
       </c>
       <c r="F129" s="3"/>
       <c r="I129" s="4"/>
-      <c r="L129" t="s">
+      <c r="L129" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -4997,7 +5004,7 @@
         <v>415</v>
       </c>
       <c r="L130" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -5017,7 +5024,7 @@
       <c r="H131" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L131" t="s">
+      <c r="L131" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5039,7 +5046,7 @@
         <v>17</v>
       </c>
       <c r="I132" s="36"/>
-      <c r="L132" t="s">
+      <c r="L132" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5059,7 +5066,7 @@
       <c r="H133" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L133" t="s">
+      <c r="L133" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5086,7 +5093,7 @@
       <c r="K134" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="L134" t="s">
+      <c r="L134" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5111,7 +5118,7 @@
       <c r="K135" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="L135" t="s">
+      <c r="L135" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5131,7 +5138,7 @@
       <c r="H136" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L136" t="s">
+      <c r="L136" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5151,7 +5158,7 @@
       </c>
       <c r="H137" s="4"/>
       <c r="L137" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="138" spans="1:12">
@@ -5172,8 +5179,8 @@
         <v>17</v>
       </c>
       <c r="I138" s="36"/>
-      <c r="L138" t="s">
-        <v>505</v>
+      <c r="L138" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -5215,7 +5222,7 @@
         <v>417</v>
       </c>
       <c r="L140" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="141" spans="1:12">
@@ -5234,7 +5241,7 @@
       <c r="H141" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L141" t="s">
+      <c r="L141" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5255,7 +5262,7 @@
         <v>418</v>
       </c>
       <c r="L142" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="143" spans="1:12">
@@ -5276,7 +5283,7 @@
         <v>362</v>
       </c>
       <c r="L143" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -5295,7 +5302,7 @@
       <c r="H144" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L144" t="s">
+      <c r="L144" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5317,7 +5324,7 @@
         <v>211</v>
       </c>
       <c r="L145" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="146" spans="1:12">
@@ -5336,7 +5343,7 @@
       <c r="H146" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L146" t="s">
+      <c r="L146" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5356,7 +5363,7 @@
       <c r="H147" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L147" t="s">
+      <c r="L147" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5378,7 +5385,7 @@
         <v>17</v>
       </c>
       <c r="K148" s="7"/>
-      <c r="L148" t="s">
+      <c r="L148" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5400,7 +5407,7 @@
         <v>121</v>
       </c>
       <c r="K149" s="7"/>
-      <c r="L149" t="s">
+      <c r="L149" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5422,7 +5429,7 @@
       </c>
       <c r="K150" s="7"/>
       <c r="L150" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="151" spans="1:12">
@@ -5441,7 +5448,7 @@
       <c r="H151" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L151" t="s">
+      <c r="L151" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5455,14 +5462,16 @@
       <c r="C152" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="D152" s="3"/>
+      <c r="D152" s="3" t="s">
+        <v>504</v>
+      </c>
       <c r="E152" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H152" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L152" t="s">
+      <c r="L152" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5482,7 +5491,7 @@
       <c r="H153" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L153" t="s">
+      <c r="L153" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5523,7 +5532,7 @@
       <c r="H155" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L155" t="s">
+      <c r="L155" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5543,7 +5552,7 @@
       <c r="H156" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L156" t="s">
+      <c r="L156" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5565,7 +5574,7 @@
         <v>420</v>
       </c>
       <c r="L157" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="158" spans="1:12">
@@ -5588,7 +5597,7 @@
       </c>
       <c r="I158" s="36"/>
       <c r="K158" s="7"/>
-      <c r="L158" t="s">
+      <c r="L158" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5612,7 +5621,7 @@
       <c r="I159" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="L159" t="s">
+      <c r="L159" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5630,7 +5639,7 @@
         <v>388</v>
       </c>
       <c r="L160" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="161" spans="1:12">
@@ -5651,7 +5660,7 @@
       </c>
       <c r="K161" s="7"/>
       <c r="L161" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="162" spans="1:12">
@@ -5688,7 +5697,7 @@
       <c r="H163" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L163" t="s">
+      <c r="L163" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5708,7 +5717,7 @@
       <c r="H164" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L164" t="s">
+      <c r="L164" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5727,7 +5736,7 @@
       </c>
       <c r="H165" s="4"/>
       <c r="L165" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
     </row>
     <row r="166" spans="1:12">
@@ -5746,8 +5755,8 @@
       <c r="H166" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L166" t="s">
-        <v>503</v>
+      <c r="L166" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="167" spans="1:12">
@@ -5767,7 +5776,7 @@
         <v>363</v>
       </c>
       <c r="K167" s="7"/>
-      <c r="L167" t="s">
+      <c r="L167" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5787,7 +5796,7 @@
       <c r="H168" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L168" t="s">
+      <c r="L168" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5809,7 +5818,7 @@
         <v>17</v>
       </c>
       <c r="I169" s="36"/>
-      <c r="L169" t="s">
+      <c r="L169" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5829,7 +5838,7 @@
       <c r="H170" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="L170" t="s">
+      <c r="L170" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5849,8 +5858,8 @@
       <c r="H171" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L171" t="s">
-        <v>496</v>
+      <c r="L171" s="10" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="172" spans="1:12">
@@ -5869,7 +5878,7 @@
       <c r="H172" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L172" t="s">
+      <c r="L172" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5899,7 +5908,7 @@
         <v>462</v>
       </c>
       <c r="L173" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="174" spans="1:12">
@@ -5921,7 +5930,7 @@
       <c r="H174" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="L174" t="s">
+      <c r="L174" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5939,7 +5948,7 @@
         <v>388</v>
       </c>
       <c r="L175" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="176" spans="1:12">
@@ -5956,7 +5965,7 @@
         <v>388</v>
       </c>
       <c r="L176" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="177" spans="1:12">
@@ -5976,7 +5985,7 @@
         <v>422</v>
       </c>
       <c r="L177" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="178" spans="1:12">
@@ -5995,7 +6004,7 @@
       <c r="H178" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L178" t="s">
+      <c r="L178" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -6015,7 +6024,7 @@
       <c r="H179" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L179" t="s">
+      <c r="L179" s="10" t="s">
         <v>496</v>
       </c>
     </row>
@@ -6035,18 +6044,22 @@
       <c r="H180" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L180" t="s">
-        <v>503</v>
+      <c r="L180" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="181" spans="1:12">
       <c r="H181" s="4"/>
+      <c r="L181"/>
     </row>
     <row r="182" spans="1:12">
       <c r="H182" s="4"/>
+      <c r="L182"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L182"/>
+  <autoFilter ref="A1:L182">
+    <filterColumn colId="4"/>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C35" r:id="rId1"/>
     <hyperlink ref="F35" r:id="rId2"/>

</xml_diff>